<commit_message>
Add reports for carry increment adder
</commit_message>
<xml_diff>
--- a/Reports Screens/VLSI Project Reports.xlsx
+++ b/Reports Screens/VLSI Project Reports.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="16">
   <si>
     <t>Design Reports</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Floating Point Adder</t>
-  </si>
-  <si>
-    <t>20ns</t>
   </si>
 </sst>
 </file>
@@ -735,7 +732,7 @@
         <v>3616.9</v>
       </c>
       <c r="G7" s="20">
-        <v>333.897461</v>
+        <v>333.8</v>
       </c>
       <c r="H7" s="20">
         <v>6383.1</v>
@@ -773,7 +770,7 @@
         <v>17811.4</v>
       </c>
       <c r="U7" s="20">
-        <v>34.626087</v>
+        <v>34.62</v>
       </c>
       <c r="V7" s="20">
         <v>19998.0</v>
@@ -946,26 +943,26 @@
         <v>745.5</v>
       </c>
       <c r="H12" s="20">
-        <v>6407.1</v>
+        <v>181.8</v>
       </c>
       <c r="I12" s="19"/>
       <c r="J12" s="20">
-        <v>240.0</v>
+        <v>204.0</v>
       </c>
       <c r="K12" s="20">
-        <v>2092.1</v>
+        <v>2656.4</v>
       </c>
       <c r="L12" s="20">
-        <v>19998.0</v>
+        <v>16843.6</v>
       </c>
       <c r="M12" s="20">
-        <v>18758.3</v>
+        <v>14187.0</v>
       </c>
       <c r="N12" s="20">
-        <v>24.35</v>
+        <v>41.5</v>
       </c>
       <c r="O12" s="20">
-        <v>19998.0</v>
+        <v>2656.4</v>
       </c>
       <c r="P12" s="18"/>
       <c r="Q12" s="20">
@@ -984,7 +981,7 @@
         <v>1359.4</v>
       </c>
       <c r="V12" s="20">
-        <v>6649.1</v>
+        <v>67.6</v>
       </c>
       <c r="W12" s="21"/>
       <c r="X12" s="18"/>
@@ -1153,8 +1150,8 @@
       <c r="G17" s="20">
         <v>868.78</v>
       </c>
-      <c r="H17" s="20" t="s">
-        <v>16</v>
+      <c r="H17" s="20">
+        <v>156.7</v>
       </c>
       <c r="I17" s="19"/>
       <c r="J17" s="20">
@@ -1172,7 +1169,9 @@
       <c r="N17" s="20">
         <v>879.05</v>
       </c>
-      <c r="O17" s="20"/>
+      <c r="O17" s="20">
+        <v>155.7</v>
+      </c>
       <c r="P17" s="18"/>
       <c r="Q17" s="20">
         <v>2305.0</v>

</xml_diff>